<commit_message>
Adjustments of small typos in the documents
</commit_message>
<xml_diff>
--- a/documents/FinalEvaluation.xlsx
+++ b/documents/FinalEvaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39b1b8d5ba36f28f/Master/SemesterZwei/NLPPraktikum/PassiveToActiveWithNLP/passiveToActive/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="278" documentId="11_626586E0D94BE80E62355476585DCE3A87450968" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76072DDF-FF06-4E33-B1EE-085F12521CFA}"/>
+  <xr:revisionPtr revIDLastSave="279" documentId="11_626586E0D94BE80E62355476585DCE3A87450968" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AC0F823-CE85-471E-A3F0-B051C9CA8C69}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2460" yWindow="2460" windowWidth="14380" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinalEvaluation" sheetId="1" r:id="rId1"/>
@@ -6944,7 +6944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0974C1FA-7C99-4F1D-BB34-4C1F92DD857B}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B5" zoomScale="70" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:B16"/>
     </sheetView>
   </sheetViews>
@@ -13341,8 +13341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317B4BFB-06FF-49CF-A352-1E0603BF66C9}">
   <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J8"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>